<commit_message>
Fixed thesis and sheet with max values to rectangular beam.
</commit_message>
<xml_diff>
--- a/Solutions/FiniteElement/Beam/MaxValues/Newmark/MaxValues_FiniteElement_Beam_RectangularProfile_w0=10_wf=90_nEl=4.xlsx
+++ b/Solutions/FiniteElement/Beam/MaxValues/Newmark/MaxValues_FiniteElement_Beam_RectangularProfile_w0=10_wf=90_nEl=4.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\IC Vibrações\Solutions\FiniteElement\Beam\MaxValues\Newmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15D39D61-7192-474F-B86B-5D8E787F3A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1305B0-46DA-486A-A483-499339C8AF7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico2" sheetId="3" r:id="rId1"/>
     <sheet name="Gráfico4" sheetId="5" r:id="rId2"/>
     <sheet name="MaxValues_FiniteElement_Beam_Re" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,6 +657,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Nó 2</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1174,6 +1187,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Nó 3</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1700,6 +1716,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Nó 4</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2525,6 +2544,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Nó 1</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3052,6 +3074,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Nó 2</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3579,6 +3604,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Nó 3</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -4105,6 +4133,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Nó 4</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -4632,6 +4663,9 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>Nó 5</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -6487,7 +6521,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
@@ -6498,10 +6532,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -6512,7 +6546,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9649918" cy="6019488"/>
+    <xdr:ext cx="9649918" cy="6011680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -6545,7 +6579,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9649918" cy="6019488"/>
+    <xdr:ext cx="9647115" cy="6008077"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -6870,11 +6904,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="K1:O81 A1:A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10291,23 +10325,23 @@
         <v>0</v>
       </c>
       <c r="K66">
-        <f t="shared" ref="K66:K101" si="6">DEGREES(E66)</f>
+        <f t="shared" ref="K66:K81" si="6">DEGREES(E66)</f>
         <v>6.6133954485481237</v>
       </c>
       <c r="L66">
-        <f t="shared" ref="L66:L101" si="7">DEGREES(F66)</f>
+        <f t="shared" ref="L66:L81" si="7">DEGREES(F66)</f>
         <v>4.4299490202797331</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M101" si="8">DEGREES(G66)</f>
+        <f t="shared" ref="M66:M81" si="8">DEGREES(G66)</f>
         <v>6.4778357197366984E-11</v>
       </c>
       <c r="N66">
-        <f t="shared" ref="N66:N101" si="9">DEGREES(H66)</f>
+        <f t="shared" ref="N66:N81" si="9">DEGREES(H66)</f>
         <v>4.4299490202780207</v>
       </c>
       <c r="O66">
-        <f t="shared" ref="O66:O101" si="10">DEGREES(I66)</f>
+        <f t="shared" ref="O66:O81" si="10">DEGREES(I66)</f>
         <v>6.6133954485533373</v>
       </c>
     </row>

</xml_diff>